<commit_message>
xlsx files were changed to csv files
</commit_message>
<xml_diff>
--- a/AIS/SPARC4_Spectral_Response/Channel 3/ccd.xlsx
+++ b/AIS/SPARC4_Spectral_Response/Channel 3/ccd.xlsx
@@ -260,10 +260,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B18"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.68359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.83"/>
   </cols>

</xml_diff>